<commit_message>
Including PUT methods Test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Siva\Automation\Intellij\APIAutomationJava\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931D4F78-1D45-4E46-88A0-3E835066C1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30334CFC-73BC-4F26-BAA7-D2CFEE518A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Testcase</t>
   </si>
@@ -33,18 +33,9 @@
     <t>Execute</t>
   </si>
   <si>
-    <t>Body</t>
-  </si>
-  <si>
-    <t>Expected Code</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>End</t>
   </si>
   <si>
@@ -60,7 +51,29 @@
     <t>POST_CreateTourist</t>
   </si>
   <si>
-    <t>{ "tourist_name": "Mike", "tourist_email": "mike4567@gmail.com","tourist_location": "Paris"}</t>
+    <t>Input1</t>
+  </si>
+  <si>
+    <t>Input2</t>
+  </si>
+  <si>
+    <t>PUT_UpdateTourist</t>
+  </si>
+  <si>
+    <t>Input3</t>
+  </si>
+  <si>
+    <t>{ "tourist_name": "Mike", "tourist_email": "mhi2ke4567341@gmail.com","tourist_location": "Paris"}</t>
+  </si>
+  <si>
+    <t>{ "tourist_name": "Mike", "tourist_email": "mikqqee12eaaqqqaaaaa1a12aaaaae456977341@gmail.com","tourist_location": "Paris"}</t>
+  </si>
+  <si>
+    <t>{"tourist_name": "Mike Update",
+ "tourist_email": "miksqqqqqssss12se123@gmail.com","tourist_location": "Paris"}</t>
+  </si>
+  <si>
+    <t>122849</t>
   </si>
 </sst>
 </file>
@@ -382,19 +395,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="3" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,44 +415,67 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
+      <c r="F4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>